<commit_message>
Minimal changes to the documentation file, new links.
</commit_message>
<xml_diff>
--- a/Documentation/Projekt MUM 2020 - rozpiska.xlsx
+++ b/Documentation/Projekt MUM 2020 - rozpiska.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="134">
   <si>
     <t>Zadanie</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>TERMIN 15.05.20 - 20:00</t>
+  </si>
+  <si>
+    <t>Obsługa uchwytu</t>
+  </si>
+  <si>
+    <t>https://www.skyatnightmagazine.com/advice/how-to-set-up-an-equatorial-mount/</t>
   </si>
 </sst>
 </file>
@@ -668,7 +674,7 @@
     <xdr:ext cx="4191000" cy="11430000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -696,7 +702,7 @@
     <xdr:ext cx="7048500" cy="3514725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -724,7 +730,7 @@
     <xdr:ext cx="2857500" cy="2638425"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -752,7 +758,7 @@
     <xdr:ext cx="2981325" cy="3219450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1781,6 +1787,14 @@
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
     </row>
+    <row r="148">
+      <c r="A148" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E5"/>
@@ -1806,7 +1820,8 @@
     <hyperlink r:id="rId21" ref="B98"/>
     <hyperlink r:id="rId22" ref="D102"/>
     <hyperlink r:id="rId23" ref="D106"/>
+    <hyperlink r:id="rId24" ref="B148"/>
   </hyperlinks>
-  <drawing r:id="rId24"/>
+  <drawing r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>